<commit_message>
Communications and Electrical data updated
Mistake in calculating the average values rectified.
</commit_message>
<xml_diff>
--- a/Intern Project/World_Poverty_Analysis/RBI_Data/World_Power_and_communications_comparison.xlsx
+++ b/Intern Project/World_Poverty_Analysis/RBI_Data/World_Power_and_communications_comparison.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="251">
   <si>
     <t>Electric power</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t>Euro area</t>
+  </si>
+  <si>
+    <t>World's Average</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1258,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1279,9 +1282,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1621,10 +1621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L241"/>
+  <dimension ref="A1:M260"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A226" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D243" sqref="D243"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A212" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A239" sqref="A239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9520,7 +9520,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="209" spans="1:12">
+    <row r="209" spans="1:13">
       <c r="A209" s="3" t="s">
         <v>226</v>
       </c>
@@ -9558,7 +9558,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="210" spans="1:12">
+    <row r="210" spans="1:13">
       <c r="A210" s="3" t="s">
         <v>227</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="211" spans="1:12">
+    <row r="211" spans="1:13">
       <c r="A211" s="3" t="s">
         <v>228</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="212" spans="1:12">
+    <row r="212" spans="1:13">
       <c r="A212" s="3" t="s">
         <v>229</v>
       </c>
@@ -9672,7 +9672,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="213" spans="1:12">
+    <row r="213" spans="1:13">
       <c r="A213" s="3" t="s">
         <v>230</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="214" spans="1:12">
+    <row r="214" spans="1:13">
       <c r="A214" s="3" t="s">
         <v>231</v>
       </c>
@@ -9748,7 +9748,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="215" spans="1:12">
+    <row r="215" spans="1:13">
       <c r="A215" s="3" t="s">
         <v>232</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="216" spans="1:12">
+    <row r="216" spans="1:13">
       <c r="A216" s="3" t="s">
         <v>233</v>
       </c>
@@ -9824,7 +9824,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="217" spans="1:12">
+    <row r="217" spans="1:13">
       <c r="A217" s="3" t="s">
         <v>234</v>
       </c>
@@ -9862,7 +9862,7 @@
         <v>4219</v>
       </c>
     </row>
-    <row r="218" spans="1:12">
+    <row r="218" spans="1:13">
       <c r="A218" s="3" t="s">
         <v>235</v>
       </c>
@@ -9900,540 +9900,58 @@
         <v>2742</v>
       </c>
     </row>
-    <row r="219" spans="1:12">
-      <c r="A219" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="B219" s="6">
-        <v>3044</v>
-      </c>
-      <c r="C219" s="3">
-        <v>8</v>
-      </c>
-      <c r="D219" s="3">
-        <v>17</v>
-      </c>
-      <c r="E219" s="3">
-        <v>89</v>
-      </c>
-      <c r="F219" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G219" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H219" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I219" s="3">
-        <v>10.4</v>
-      </c>
-      <c r="J219" s="3">
-        <v>14.6</v>
-      </c>
-      <c r="K219" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="L219" s="6">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="220" spans="1:12">
-      <c r="A220" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="B220" s="3">
-        <v>233</v>
-      </c>
-      <c r="C220" s="3">
-        <v>15</v>
-      </c>
-      <c r="D220" s="3">
-        <v>1</v>
-      </c>
-      <c r="E220" s="3">
-        <v>47</v>
-      </c>
-      <c r="F220" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G220" s="3">
-        <v>42</v>
-      </c>
-      <c r="H220" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I220" s="3">
-        <v>8.9</v>
-      </c>
-      <c r="J220" s="3">
-        <v>11.9</v>
-      </c>
-      <c r="K220" s="4">
-        <v>5</v>
-      </c>
-      <c r="L220" s="6">
-        <v>3462</v>
-      </c>
-    </row>
-    <row r="221" spans="1:12">
-      <c r="A221" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="B221" s="6">
-        <v>1816</v>
-      </c>
-      <c r="C221" s="3">
-        <v>10</v>
-      </c>
-      <c r="D221" s="3">
-        <v>12</v>
-      </c>
-      <c r="E221" s="3">
-        <v>88</v>
-      </c>
-      <c r="F221" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G221" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H221" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I221" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="J221" s="3">
-        <v>13.1</v>
-      </c>
-      <c r="K221" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="L221" s="6">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="222" spans="1:12">
-      <c r="A222" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B222" s="3">
-        <v>734</v>
-      </c>
-      <c r="C222" s="3">
-        <v>16</v>
-      </c>
-      <c r="D222" s="3">
-        <v>5</v>
-      </c>
-      <c r="E222" s="3">
-        <v>83</v>
-      </c>
-      <c r="F222" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G222" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H222" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I222" s="3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="J222" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="K222" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="L222" s="6">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="223" spans="1:12">
-      <c r="A223" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B223" s="6">
-        <v>2932</v>
-      </c>
-      <c r="C223" s="3">
-        <v>9</v>
-      </c>
-      <c r="D223" s="3">
-        <v>19</v>
-      </c>
-      <c r="E223" s="3">
-        <v>92</v>
-      </c>
-      <c r="F223" s="3">
-        <v>27</v>
-      </c>
-      <c r="G223" s="3">
-        <v>9</v>
-      </c>
-      <c r="H223" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I223" s="3">
-        <v>9.4</v>
-      </c>
-      <c r="J223" s="3">
-        <v>14.9</v>
-      </c>
-      <c r="K223" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="L223" s="6">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="224" spans="1:12">
-      <c r="A224" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="B224" s="6">
-        <v>1646</v>
-      </c>
-      <c r="C224" s="3">
-        <v>10</v>
-      </c>
-      <c r="D224" s="3">
-        <v>11</v>
-      </c>
-      <c r="E224" s="3">
-        <v>82</v>
-      </c>
-      <c r="F224" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G224" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H224" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I224" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="J224" s="3">
-        <v>12.6</v>
-      </c>
-      <c r="K224" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="L224" s="6">
-        <v>1739</v>
-      </c>
-    </row>
-    <row r="225" spans="1:12">
-      <c r="A225" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B225" s="6">
-        <v>2582</v>
-      </c>
-      <c r="C225" s="3">
-        <v>6</v>
-      </c>
-      <c r="D225" s="3">
-        <v>17</v>
-      </c>
-      <c r="E225" s="3">
-        <v>89</v>
-      </c>
-      <c r="F225" s="3">
-        <v>6</v>
-      </c>
-      <c r="G225" s="3">
-        <v>2</v>
-      </c>
-      <c r="H225" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I225" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="J225" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="K225" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L225" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="226" spans="1:12">
-      <c r="A226" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B226" s="6">
-        <v>2951</v>
-      </c>
-      <c r="C226" s="3">
-        <v>12</v>
-      </c>
-      <c r="D226" s="3">
-        <v>21</v>
-      </c>
-      <c r="E226" s="3">
-        <v>108</v>
-      </c>
-      <c r="F226" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G226" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H226" s="4">
-        <v>99</v>
-      </c>
-      <c r="I226" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="J226" s="3">
-        <v>12.5</v>
-      </c>
-      <c r="K226" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="L226" s="3">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="227" spans="1:12">
-      <c r="A227" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B227" s="6">
-        <v>1985</v>
-      </c>
-      <c r="C227" s="3">
-        <v>15</v>
-      </c>
-      <c r="D227" s="3">
-        <v>18</v>
-      </c>
-      <c r="E227" s="3">
-        <v>108</v>
-      </c>
-      <c r="F227" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G227" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H227" s="3">
-        <v>99</v>
-      </c>
-      <c r="I227" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="J227" s="3">
-        <v>14.9</v>
-      </c>
-      <c r="K227" s="3">
-        <v>3</v>
-      </c>
-      <c r="L227" s="6">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="228" spans="1:12">
-      <c r="A228" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B228" s="6">
-        <v>1696</v>
-      </c>
-      <c r="C228" s="3">
-        <v>15</v>
-      </c>
-      <c r="D228" s="3">
-        <v>16</v>
-      </c>
-      <c r="E228" s="3">
-        <v>95</v>
-      </c>
-      <c r="F228" s="3">
-        <v>27</v>
-      </c>
-      <c r="G228" s="4">
-        <v>57</v>
-      </c>
-      <c r="H228" s="3">
-        <v>97</v>
-      </c>
-      <c r="I228" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="J228" s="3">
-        <v>10.9</v>
-      </c>
-      <c r="K228" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="L228" s="6">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12">
-      <c r="A229" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="B229" s="3">
-        <v>605</v>
-      </c>
-      <c r="C229" s="3">
-        <v>20</v>
-      </c>
-      <c r="D229" s="3">
-        <v>3</v>
-      </c>
-      <c r="E229" s="3">
-        <v>69</v>
-      </c>
-      <c r="F229" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G229" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H229" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I229" s="3">
-        <v>3</v>
-      </c>
-      <c r="J229" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="K229" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L229" s="6">
-        <v>1823</v>
-      </c>
-    </row>
-    <row r="230" spans="1:12">
-      <c r="A230" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="B230" s="3">
-        <v>535</v>
-      </c>
-      <c r="C230" s="3">
-        <v>11</v>
-      </c>
-      <c r="D230" s="3">
-        <v>1</v>
-      </c>
-      <c r="E230" s="3">
-        <v>59</v>
-      </c>
-      <c r="F230" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G230" s="4">
-        <v>23</v>
-      </c>
-      <c r="H230" s="3">
-        <v>84</v>
-      </c>
-      <c r="I230" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="J230" s="3">
-        <v>14.6</v>
-      </c>
-      <c r="K230" s="4">
-        <v>3.3</v>
-      </c>
-      <c r="L230" s="6">
-        <v>4294</v>
-      </c>
-    </row>
-    <row r="231" spans="1:12">
-      <c r="A231" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="B231" s="6">
-        <v>8896</v>
-      </c>
-      <c r="C231" s="3">
-        <v>6</v>
-      </c>
-      <c r="D231" s="3">
-        <v>44</v>
-      </c>
-      <c r="E231" s="3">
-        <v>123</v>
-      </c>
-      <c r="F231" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G231" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H231" s="3">
-        <v>100</v>
-      </c>
-      <c r="I231" s="3">
-        <v>25.2</v>
-      </c>
-      <c r="J231" s="3">
-        <v>20.6</v>
-      </c>
-      <c r="K231" s="3">
-        <v>2.7</v>
-      </c>
-      <c r="L231" s="3">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="232" spans="1:12">
-      <c r="A232" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="B232" s="6">
-        <v>6599</v>
-      </c>
-      <c r="C232" s="3">
-        <v>6</v>
-      </c>
-      <c r="D232" s="3">
-        <v>48</v>
-      </c>
-      <c r="E232" s="3">
-        <v>120</v>
-      </c>
-      <c r="F232" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G232" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H232" s="3">
-        <v>99</v>
-      </c>
-      <c r="I232" s="3">
-        <v>27.8</v>
-      </c>
-      <c r="J232" s="3">
-        <v>25.2</v>
-      </c>
-      <c r="K232" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="L232" s="3">
-        <v>824</v>
-      </c>
+    <row r="219" spans="1:13">
+      <c r="B219" s="5"/>
+    </row>
+    <row r="220" spans="1:13">
+      <c r="B220" s="5">
+        <f>AVERAGE(B6:B219)</f>
+        <v>4290.6940298507461</v>
+      </c>
+      <c r="C220" s="5">
+        <f t="shared" ref="C220:M220" si="0">AVERAGE(C6:C219)</f>
+        <v>13.111940298507463</v>
+      </c>
+      <c r="D220" s="5">
+        <f t="shared" si="0"/>
+        <v>20.215686274509803</v>
+      </c>
+      <c r="E220" s="5">
+        <f t="shared" si="0"/>
+        <v>99.97</v>
+      </c>
+      <c r="F220" s="5">
+        <f t="shared" si="0"/>
+        <v>171.51401869158877</v>
+      </c>
+      <c r="G220" s="5">
+        <f t="shared" si="0"/>
+        <v>153.26363636363635</v>
+      </c>
+      <c r="H220" s="5">
+        <f t="shared" si="0"/>
+        <v>94.105633802816897</v>
+      </c>
+      <c r="I220" s="5">
+        <f t="shared" si="0"/>
+        <v>14.21875</v>
+      </c>
+      <c r="J220" s="5">
+        <f t="shared" si="0"/>
+        <v>17.724431818181817</v>
+      </c>
+      <c r="K220" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4724637681159409</v>
+      </c>
+      <c r="L220" s="5">
+        <f t="shared" si="0"/>
+        <v>1671.4028776978416</v>
+      </c>
+      <c r="M220" s="5"/>
     </row>
     <row r="234" spans="1:12">
-      <c r="A234" s="11"/>
+      <c r="A234" s="10"/>
     </row>
     <row r="236" spans="1:12" ht="30">
       <c r="A236" s="2"/>
@@ -10472,50 +9990,52 @@
       </c>
     </row>
     <row r="238" spans="1:12">
-      <c r="A238" s="10"/>
+      <c r="A238" t="s">
+        <v>250</v>
+      </c>
       <c r="B238" s="5">
-        <f>AVERAGE(B6:B232)</f>
-        <v>4129.7770270270266</v>
+        <f>AVERAGE(B24:B237)</f>
+        <v>4296.2901953646406</v>
       </c>
       <c r="C238" s="5">
-        <f>AVERAGE(C6:C232)</f>
-        <v>12.945945945945946</v>
+        <f t="shared" ref="C238" si="1">AVERAGE(C24:C237)</f>
+        <v>13.212292197548841</v>
       </c>
       <c r="D238" s="5">
-        <f>AVERAGE(D6:D232)</f>
-        <v>19.986238532110093</v>
+        <f t="shared" ref="D238" si="2">AVERAGE(D24:D237)</f>
+        <v>19.45569885708294</v>
       </c>
       <c r="E238" s="5">
-        <f>AVERAGE(E6:E232)</f>
-        <v>99.280373831775705</v>
+        <f t="shared" ref="E238" si="3">AVERAGE(E24:E237)</f>
+        <v>98.847663043478263</v>
       </c>
       <c r="F238" s="5">
-        <f>AVERAGE(F6:F232)</f>
-        <v>167.38181818181818</v>
+        <f t="shared" ref="F238" si="4">AVERAGE(F24:F237)</f>
+        <v>174.07514018691589</v>
       </c>
       <c r="G238" s="5">
-        <f t="shared" ref="G238:L238" si="0">AVERAGE(G6:G232)</f>
-        <v>147.75652173913045</v>
+        <f t="shared" ref="G238" si="5">AVERAGE(G24:G237)</f>
+        <v>135.48330419580418</v>
       </c>
       <c r="H238" s="5">
-        <f t="shared" si="0"/>
-        <v>94.195945945945951</v>
+        <f t="shared" ref="H238" si="6">AVERAGE(H24:H237)</f>
+        <v>93.56235102925244</v>
       </c>
       <c r="I238" s="5">
-        <f t="shared" si="0"/>
-        <v>13.884210526315789</v>
+        <f t="shared" ref="I238" si="7">AVERAGE(I24:I237)</f>
+        <v>14.315547839506168</v>
       </c>
       <c r="J238" s="5">
-        <f t="shared" si="0"/>
-        <v>17.405263157894733</v>
+        <f t="shared" ref="J238" si="8">AVERAGE(J24:J237)</f>
+        <v>17.602002665544333</v>
       </c>
       <c r="K238" s="5">
-        <f t="shared" si="0"/>
-        <v>3.4026315789473673</v>
+        <f t="shared" ref="K238" si="9">AVERAGE(K24:K237)</f>
+        <v>3.4935348731884042</v>
       </c>
       <c r="L238" s="5">
-        <f t="shared" si="0"/>
-        <v>1674.3157894736842</v>
+        <f t="shared" ref="L238" si="10">AVERAGE(L24:L237)</f>
+        <v>1770.8390849820144</v>
       </c>
     </row>
     <row r="239" spans="1:12">
@@ -10557,6 +10077,538 @@
       </c>
       <c r="L241" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12">
+      <c r="A247" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B247" s="6">
+        <v>3044</v>
+      </c>
+      <c r="C247" s="3">
+        <v>8</v>
+      </c>
+      <c r="D247" s="3">
+        <v>17</v>
+      </c>
+      <c r="E247" s="3">
+        <v>89</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G247" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H247" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I247" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="J247" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="K247" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="L247" s="6">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12">
+      <c r="A248" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B248" s="3">
+        <v>233</v>
+      </c>
+      <c r="C248" s="3">
+        <v>15</v>
+      </c>
+      <c r="D248" s="3">
+        <v>1</v>
+      </c>
+      <c r="E248" s="3">
+        <v>47</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G248" s="3">
+        <v>42</v>
+      </c>
+      <c r="H248" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I248" s="3">
+        <v>8.9</v>
+      </c>
+      <c r="J248" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="K248" s="4">
+        <v>5</v>
+      </c>
+      <c r="L248" s="6">
+        <v>3462</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12">
+      <c r="A249" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B249" s="6">
+        <v>1816</v>
+      </c>
+      <c r="C249" s="3">
+        <v>10</v>
+      </c>
+      <c r="D249" s="3">
+        <v>12</v>
+      </c>
+      <c r="E249" s="3">
+        <v>88</v>
+      </c>
+      <c r="F249" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H249" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I249" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="J249" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="K249" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L249" s="6">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12">
+      <c r="A250" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B250" s="3">
+        <v>734</v>
+      </c>
+      <c r="C250" s="3">
+        <v>16</v>
+      </c>
+      <c r="D250" s="3">
+        <v>5</v>
+      </c>
+      <c r="E250" s="3">
+        <v>83</v>
+      </c>
+      <c r="F250" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G250" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H250" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I250" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J250" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="K250" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="L250" s="6">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12">
+      <c r="A251" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B251" s="6">
+        <v>2932</v>
+      </c>
+      <c r="C251" s="3">
+        <v>9</v>
+      </c>
+      <c r="D251" s="3">
+        <v>19</v>
+      </c>
+      <c r="E251" s="3">
+        <v>92</v>
+      </c>
+      <c r="F251" s="3">
+        <v>27</v>
+      </c>
+      <c r="G251" s="3">
+        <v>9</v>
+      </c>
+      <c r="H251" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I251" s="3">
+        <v>9.4</v>
+      </c>
+      <c r="J251" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="K251" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L251" s="6">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12">
+      <c r="A252" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B252" s="6">
+        <v>1646</v>
+      </c>
+      <c r="C252" s="3">
+        <v>10</v>
+      </c>
+      <c r="D252" s="3">
+        <v>11</v>
+      </c>
+      <c r="E252" s="3">
+        <v>82</v>
+      </c>
+      <c r="F252" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G252" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H252" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I252" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="J252" s="3">
+        <v>12.6</v>
+      </c>
+      <c r="K252" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L252" s="6">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12">
+      <c r="A253" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B253" s="6">
+        <v>2582</v>
+      </c>
+      <c r="C253" s="3">
+        <v>6</v>
+      </c>
+      <c r="D253" s="3">
+        <v>17</v>
+      </c>
+      <c r="E253" s="3">
+        <v>89</v>
+      </c>
+      <c r="F253" s="3">
+        <v>6</v>
+      </c>
+      <c r="G253" s="3">
+        <v>2</v>
+      </c>
+      <c r="H253" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I253" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="J253" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="K253" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L253" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12">
+      <c r="A254" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B254" s="6">
+        <v>2951</v>
+      </c>
+      <c r="C254" s="3">
+        <v>12</v>
+      </c>
+      <c r="D254" s="3">
+        <v>21</v>
+      </c>
+      <c r="E254" s="3">
+        <v>108</v>
+      </c>
+      <c r="F254" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G254" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H254" s="4">
+        <v>99</v>
+      </c>
+      <c r="I254" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="J254" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="K254" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="L254" s="3">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12">
+      <c r="A255" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B255" s="6">
+        <v>1985</v>
+      </c>
+      <c r="C255" s="3">
+        <v>15</v>
+      </c>
+      <c r="D255" s="3">
+        <v>18</v>
+      </c>
+      <c r="E255" s="3">
+        <v>108</v>
+      </c>
+      <c r="F255" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G255" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H255" s="3">
+        <v>99</v>
+      </c>
+      <c r="I255" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="J255" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="K255" s="3">
+        <v>3</v>
+      </c>
+      <c r="L255" s="6">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12">
+      <c r="A256" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B256" s="6">
+        <v>1696</v>
+      </c>
+      <c r="C256" s="3">
+        <v>15</v>
+      </c>
+      <c r="D256" s="3">
+        <v>16</v>
+      </c>
+      <c r="E256" s="3">
+        <v>95</v>
+      </c>
+      <c r="F256" s="3">
+        <v>27</v>
+      </c>
+      <c r="G256" s="4">
+        <v>57</v>
+      </c>
+      <c r="H256" s="3">
+        <v>97</v>
+      </c>
+      <c r="I256" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="J256" s="3">
+        <v>10.9</v>
+      </c>
+      <c r="K256" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="L256" s="6">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
+      <c r="A257" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B257" s="3">
+        <v>605</v>
+      </c>
+      <c r="C257" s="3">
+        <v>20</v>
+      </c>
+      <c r="D257" s="3">
+        <v>3</v>
+      </c>
+      <c r="E257" s="3">
+        <v>69</v>
+      </c>
+      <c r="F257" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G257" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H257" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I257" s="3">
+        <v>3</v>
+      </c>
+      <c r="J257" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="K257" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L257" s="6">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
+      <c r="A258" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B258" s="3">
+        <v>535</v>
+      </c>
+      <c r="C258" s="3">
+        <v>11</v>
+      </c>
+      <c r="D258" s="3">
+        <v>1</v>
+      </c>
+      <c r="E258" s="3">
+        <v>59</v>
+      </c>
+      <c r="F258" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G258" s="4">
+        <v>23</v>
+      </c>
+      <c r="H258" s="3">
+        <v>84</v>
+      </c>
+      <c r="I258" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="J258" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="K258" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="L258" s="6">
+        <v>4294</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
+      <c r="A259" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B259" s="6">
+        <v>8896</v>
+      </c>
+      <c r="C259" s="3">
+        <v>6</v>
+      </c>
+      <c r="D259" s="3">
+        <v>44</v>
+      </c>
+      <c r="E259" s="3">
+        <v>123</v>
+      </c>
+      <c r="F259" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G259" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H259" s="3">
+        <v>100</v>
+      </c>
+      <c r="I259" s="3">
+        <v>25.2</v>
+      </c>
+      <c r="J259" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="K259" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="L259" s="3">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12">
+      <c r="A260" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B260" s="6">
+        <v>6599</v>
+      </c>
+      <c r="C260" s="3">
+        <v>6</v>
+      </c>
+      <c r="D260" s="3">
+        <v>48</v>
+      </c>
+      <c r="E260" s="3">
+        <v>120</v>
+      </c>
+      <c r="F260" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G260" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H260" s="3">
+        <v>99</v>
+      </c>
+      <c r="I260" s="3">
+        <v>27.8</v>
+      </c>
+      <c r="J260" s="3">
+        <v>25.2</v>
+      </c>
+      <c r="K260" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="L260" s="3">
+        <v>824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>